<commit_message>
Bug fixes and report enhancements
</commit_message>
<xml_diff>
--- a/templates/template.xlsx
+++ b/templates/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SoftwareAG107\IntegrationServer\instances\default\packages\WxDevTools\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wMServiceDesigner11\IntegrationServer\packages\WxPreUpgradeAnalyzer\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D866E51-DCE3-4D7A-BA24-BD2F360E982B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E328D190-404F-4DCA-B3FA-BE3E72A8C7EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="1400" windowWidth="27290" windowHeight="11380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11150" yWindow="4340" windowWidth="21820" windowHeight="8420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -89,20 +89,20 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>314325</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1444355</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>790575</xdr:rowOff>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>67115</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88340EF7-40A9-4830-E58F-98B4C366A155}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -124,8 +124,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="314325"/>
-          <a:ext cx="2720705" cy="476250"/>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1536700" cy="1146615"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -138,9 +138,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -178,9 +178,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -213,26 +213,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -265,26 +248,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -460,9 +426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>